<commit_message>
Added data augmentation controls: flat rotation and add a plane to the scene
</commit_message>
<xml_diff>
--- a/Project Timeline.xlsx
+++ b/Project Timeline.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Grad School\Spring 2024\Thesis\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\saaso\Desktop\MachineVisionAR\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E9181054-EB8C-4EB8-B45B-61C0B6ACC0BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D335816-74A4-4491-9199-003ACD539A4A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{DC1B3FFF-4C9B-4FAD-B951-12C838A3EFAE}"/>
+    <workbookView xWindow="30612" yWindow="828" windowWidth="30936" windowHeight="17496" xr2:uid="{DC1B3FFF-4C9B-4FAD-B951-12C838A3EFAE}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -338,9 +338,6 @@
     <t>Test and record results of model</t>
   </si>
   <si>
-    <t>3D tracking model over actual object</t>
-  </si>
-  <si>
     <t>Begin developing AR remote assistance platform</t>
   </si>
   <si>
@@ -369,6 +366,9 @@
   </si>
   <si>
     <t>What Is Needed</t>
+  </si>
+  <si>
+    <t>3D tracking model over actual object (Image Segmentation)</t>
   </si>
 </sst>
 </file>
@@ -542,49 +542,16 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -595,6 +562,39 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -920,7 +920,7 @@
   <dimension ref="A1:D28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="D10" sqref="D10:D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="48.7109375" defaultRowHeight="24.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -931,21 +931,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="24.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="19" t="s">
+      <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="20" t="s">
+      <c r="B1" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="20" t="s">
+      <c r="C1" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="20" t="s">
-        <v>46</v>
+      <c r="D1" s="9" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="8" t="s">
+      <c r="A2" s="18" t="s">
         <v>3</v>
       </c>
       <c r="B2" s="1" t="s">
@@ -959,7 +959,7 @@
       </c>
     </row>
     <row r="3" spans="1:4" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="9"/>
+      <c r="A3" s="19"/>
       <c r="B3" s="1" t="s">
         <v>30</v>
       </c>
@@ -971,7 +971,7 @@
       </c>
     </row>
     <row r="4" spans="1:4" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="9"/>
+      <c r="A4" s="19"/>
       <c r="B4" s="1" t="s">
         <v>31</v>
       </c>
@@ -983,9 +983,9 @@
       </c>
     </row>
     <row r="5" spans="1:4" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="9"/>
-      <c r="B5" s="6"/>
-      <c r="C5" s="6" t="s">
+      <c r="A5" s="19"/>
+      <c r="B5" s="3"/>
+      <c r="C5" s="3" t="s">
         <v>25</v>
       </c>
       <c r="D5" s="1" t="s">
@@ -993,234 +993,232 @@
       </c>
     </row>
     <row r="6" spans="1:4" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="9"/>
-      <c r="B6" s="6"/>
-      <c r="C6" s="6"/>
+      <c r="A6" s="19"/>
+      <c r="B6" s="3"/>
+      <c r="C6" s="3"/>
       <c r="D6" s="1" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="24.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="10"/>
-      <c r="B7" s="7"/>
-      <c r="C7" s="7"/>
+      <c r="A7" s="20"/>
+      <c r="B7" s="4"/>
+      <c r="C7" s="4"/>
       <c r="D7" s="2" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="8" t="s">
+      <c r="A8" s="18" t="s">
         <v>4</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="C8" s="3"/>
-      <c r="D8" s="3"/>
+      <c r="C8" s="1"/>
+      <c r="D8" s="1"/>
     </row>
     <row r="9" spans="1:4" ht="24.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="10"/>
+      <c r="A9" s="20"/>
       <c r="B9" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="C9" s="4"/>
-      <c r="D9" s="4"/>
+      <c r="C9" s="2"/>
+      <c r="D9" s="2"/>
     </row>
     <row r="10" spans="1:4" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="8" t="s">
+      <c r="A10" s="18" t="s">
         <v>5</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="C10" s="3"/>
-      <c r="D10" s="3"/>
+      <c r="C10" s="12"/>
+      <c r="D10" s="12"/>
     </row>
     <row r="11" spans="1:4" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="9"/>
+      <c r="A11" s="19"/>
       <c r="B11" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="C11" s="5"/>
-      <c r="D11" s="5"/>
+      <c r="C11" s="17"/>
+      <c r="D11" s="17"/>
     </row>
     <row r="12" spans="1:4" ht="24.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="10"/>
+      <c r="A12" s="20"/>
       <c r="B12" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="C12" s="13"/>
+      <c r="D12" s="13"/>
+    </row>
+    <row r="13" spans="1:4" ht="24.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B13" s="2" t="s">
         <v>36</v>
-      </c>
-      <c r="C12" s="4"/>
-      <c r="D12" s="4"/>
-    </row>
-    <row r="13" spans="1:4" ht="24.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="11" t="s">
-        <v>6</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>37</v>
       </c>
       <c r="C13" s="2"/>
       <c r="D13" s="2"/>
     </row>
     <row r="14" spans="1:4" ht="24.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="11" t="s">
+      <c r="A14" s="5" t="s">
         <v>7</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C14" s="2"/>
       <c r="D14" s="2"/>
     </row>
     <row r="15" spans="1:4" ht="24.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="11" t="s">
+      <c r="A15" s="5" t="s">
         <v>8</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C15" s="2"/>
       <c r="D15" s="2"/>
     </row>
     <row r="16" spans="1:4" ht="24.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="11" t="s">
+      <c r="A16" s="5" t="s">
         <v>9</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C16" s="2"/>
       <c r="D16" s="2"/>
     </row>
     <row r="17" spans="1:4" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="12" t="s">
+      <c r="A17" s="10" t="s">
         <v>10</v>
       </c>
       <c r="B17" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C17" s="12"/>
+      <c r="D17" s="12"/>
+    </row>
+    <row r="18" spans="1:4" ht="24.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="11"/>
+      <c r="B18" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="C17" s="3"/>
-      <c r="D17" s="3"/>
-    </row>
-    <row r="18" spans="1:4" ht="24.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="13"/>
-      <c r="B18" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="C18" s="4"/>
-      <c r="D18" s="4"/>
+      <c r="C18" s="13"/>
+      <c r="D18" s="13"/>
     </row>
     <row r="19" spans="1:4" ht="24.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="11" t="s">
+      <c r="A19" s="5" t="s">
         <v>11</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C19" s="2"/>
       <c r="D19" s="2"/>
     </row>
     <row r="20" spans="1:4" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="15" t="s">
+      <c r="A20" s="14" t="s">
         <v>12</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="C20" s="3"/>
-      <c r="D20" s="3"/>
+        <v>37</v>
+      </c>
+      <c r="C20" s="12"/>
+      <c r="D20" s="12"/>
     </row>
     <row r="21" spans="1:4" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="16"/>
+      <c r="A21" s="15"/>
       <c r="B21" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C21" s="17"/>
+      <c r="D21" s="17"/>
+    </row>
+    <row r="22" spans="1:4" ht="24.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="16"/>
+      <c r="B22" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="C21" s="5"/>
-      <c r="D21" s="5"/>
-    </row>
-    <row r="22" spans="1:4" ht="24.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="17"/>
-      <c r="B22" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="C22" s="4"/>
-      <c r="D22" s="4"/>
+      <c r="C22" s="13"/>
+      <c r="D22" s="13"/>
     </row>
     <row r="23" spans="1:4" ht="24.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="18" t="s">
+      <c r="A23" s="7" t="s">
         <v>13</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C23" s="2"/>
       <c r="D23" s="2"/>
     </row>
     <row r="24" spans="1:4" ht="24.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="18" t="s">
+      <c r="A24" s="7" t="s">
         <v>14</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C24" s="2"/>
       <c r="D24" s="2"/>
     </row>
     <row r="25" spans="1:4" ht="24.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="18" t="s">
+      <c r="A25" s="7" t="s">
         <v>15</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C25" s="2"/>
       <c r="D25" s="2"/>
     </row>
     <row r="26" spans="1:4" ht="24.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="14" t="s">
+      <c r="A26" s="6" t="s">
         <v>16</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C26" s="2"/>
       <c r="D26" s="2"/>
     </row>
     <row r="27" spans="1:4" ht="24.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="14" t="s">
+      <c r="A27" s="6" t="s">
         <v>17</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C27" s="2"/>
       <c r="D27" s="2"/>
     </row>
     <row r="28" spans="1:4" ht="24.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="14" t="s">
+      <c r="A28" s="6" t="s">
         <v>18</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C28" s="2"/>
       <c r="D28" s="2"/>
     </row>
   </sheetData>
-  <mergeCells count="13">
+  <mergeCells count="11">
+    <mergeCell ref="A2:A7"/>
+    <mergeCell ref="A8:A9"/>
+    <mergeCell ref="A10:A12"/>
+    <mergeCell ref="C10:C12"/>
+    <mergeCell ref="D10:D12"/>
     <mergeCell ref="A17:A18"/>
     <mergeCell ref="C17:C18"/>
     <mergeCell ref="D17:D18"/>
     <mergeCell ref="A20:A22"/>
     <mergeCell ref="C20:C22"/>
     <mergeCell ref="D20:D22"/>
-    <mergeCell ref="A2:A7"/>
-    <mergeCell ref="A8:A9"/>
-    <mergeCell ref="C8:C9"/>
-    <mergeCell ref="D8:D9"/>
-    <mergeCell ref="A10:A12"/>
-    <mergeCell ref="C10:C12"/>
-    <mergeCell ref="D10:D12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>